<commit_message>
Add build configuration and localization support for Excel Translator
- Introduce build.yaml for builder configuration
- Add Excel and ODS file parsing capabilities
- Implement CSV parsing with improved error handling
- Enhance localization files with new translations
- Update pubspec.yaml with necessary dependencies
- Refactor StringUtils for better method name sanitization
</commit_message>
<xml_diff>
--- a/example/assets/example_localizations.xlsx
+++ b/example/assets/example_localizations.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t xml:space="preserve">Cancelar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">findProduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cari Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selemente</t>
   </si>
   <si>
     <t xml:space="preserve">submit</t>
@@ -248,7 +260,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -441,10 +453,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -559,6 +571,20 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -601,58 +627,58 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update example_localizations.xlsx with new translations
</commit_message>
<xml_diff>
--- a/example/assets/example_localizations.xlsx
+++ b/example/assets/example_localizations.xlsx
@@ -128,7 +128,7 @@
     <t xml:space="preserve">Cari Product</t>
   </si>
   <si>
-    <t xml:space="preserve">selemente</t>
+    <t xml:space="preserve">Buscar Producto</t>
   </si>
   <si>
     <t xml:space="preserve">submit</t>
@@ -255,12 +255,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -456,7 +460,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -574,16 +578,16 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>